<commit_message>
modify hitgh level plan
</commit_message>
<xml_diff>
--- a/docs/HightLevelPlan.xlsx
+++ b/docs/HightLevelPlan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t xml:space="preserve">Stage</t>
   </si>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Sam</t>
   </si>
   <si>
-    <t xml:space="preserve">Sam what learn something</t>
+    <t xml:space="preserve">Sam want learn something</t>
   </si>
   <si>
     <t xml:space="preserve">A, M want to use interesting interactive interface</t>
@@ -70,12 +70,18 @@
     <t xml:space="preserve">Martin</t>
   </si>
   <si>
-    <t xml:space="preserve">Mart whant spent time with friends with passive developing</t>
+    <t xml:space="preserve">Mart want spent time with friends with passive developing</t>
   </si>
   <si>
     <t xml:space="preserve">2. Add different input formats (buttons, input text, voice etc.)</t>
   </si>
   <si>
+    <t xml:space="preserve">Vlad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disabled person</t>
+  </si>
+  <si>
     <t xml:space="preserve">2. Add plot between levels to the world, fairy tail</t>
   </si>
   <si>
@@ -127,10 +133,82 @@
     <t xml:space="preserve">Framework</t>
   </si>
   <si>
-    <t xml:space="preserve">ASM want view appropriate context to their current world</t>
-  </si>
-  <si>
     <t xml:space="preserve">BackLog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASM want to use app with mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Adaptive design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASM want differntiate each other in multiptiplayer game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Avatars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Names (Nicknames)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Identificators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. User colors for hero and for enemy (question visualisation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASM want to have different variant of game formats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.  Crossword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. True-false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Quiz (choose answer from list)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Quiz (write answer manually)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASM want to have possibility to communicate with each other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Add description to account with contacts (mail, telegram etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Voice chat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Text chat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Add Loud Phrase (user pres on button and all team members see phrase)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S want to analyse progress and use it for learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Repeat mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Compare with other players</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VS want to have accessible interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Voice interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Big font</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Keyboard first</t>
   </si>
 </sst>
 </file>
@@ -145,6 +223,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -165,12 +244,14 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -340,18 +421,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="43.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="11.54"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.54"/>
@@ -437,13 +518,19 @@
       <c r="E4" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="K4" s="0"/>
       <c r="L4" s="0"/>
       <c r="M4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K5" s="0"/>
       <c r="L5" s="0"/>
@@ -454,10 +541,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -465,59 +552,59 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E9" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -528,47 +615,135 @@
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="0"/>
+        <v>37</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="0"/>
+      <c r="C29" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0"/>
+      <c r="E30" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0"/>
+      <c r="E32" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="0"/>
+      <c r="C33" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
       <c r="B35" s="0"/>
       <c r="C35" s="0"/>
+      <c r="E35" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0"/>
       <c r="B36" s="0"/>
       <c r="C36" s="0"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
       <c r="B37" s="0"/>
-      <c r="C37" s="0"/>
+      <c r="C37" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E42" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E43" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E45" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E46" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>